<commit_message>
improvements to documentation, building floorspace, from 30 to 32 regions, renaming of batch xml files in emissions module
</commit_message>
<xml_diff>
--- a/gcam-data-system/socioeconomics-data/assumptions/GCAM3_demand_elasticities.xlsx
+++ b/gcam-data-system/socioeconomics-data/assumptions/GCAM3_demand_elasticities.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="0" windowWidth="21960" windowHeight="15140" tabRatio="500" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="1360" yWindow="0" windowWidth="21960" windowHeight="15140" tabRatio="500" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ind_calcsoutput" sheetId="9" r:id="rId1"/>
-    <sheet name="ind_calcs_GDP" sheetId="1" r:id="rId2"/>
-    <sheet name="A32.inc_elas.csv" sheetId="2" r:id="rId3"/>
-    <sheet name="cement_calcs" sheetId="7" r:id="rId4"/>
-    <sheet name="cement_calcs_output" sheetId="12" r:id="rId5"/>
-    <sheet name="A321.inc_elas_output.csv" sheetId="10" r:id="rId6"/>
-    <sheet name="A321.inc_elas.csv" sheetId="8" r:id="rId7"/>
-    <sheet name="bld_calcs" sheetId="3" r:id="rId8"/>
-    <sheet name="A42.inc_elas.csv" sheetId="4" r:id="rId9"/>
-    <sheet name="trn_calcs" sheetId="5" r:id="rId10"/>
-    <sheet name="A52.inc_elas.csv" sheetId="6" r:id="rId11"/>
+    <sheet name="A32.inc_elas.csv (2)" sheetId="13" r:id="rId2"/>
+    <sheet name="ind_calcs_GDP" sheetId="1" r:id="rId3"/>
+    <sheet name="A32.inc_elas.csv" sheetId="2" r:id="rId4"/>
+    <sheet name="cement_calcs" sheetId="7" r:id="rId5"/>
+    <sheet name="cement_calcs_output" sheetId="12" r:id="rId6"/>
+    <sheet name="A321.inc_elas_output.csv" sheetId="10" r:id="rId7"/>
+    <sheet name="A321.inc_elas.csv" sheetId="8" r:id="rId8"/>
+    <sheet name="bld_calcs" sheetId="3" r:id="rId9"/>
+    <sheet name="A42.inc_elas.csv" sheetId="4" r:id="rId10"/>
+    <sheet name="trn_calcs" sheetId="5" r:id="rId11"/>
+    <sheet name="A52.inc_elas.csv" sheetId="6" r:id="rId12"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2373" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2381" uniqueCount="88">
   <si>
     <t>Africa</t>
   </si>
@@ -273,14 +274,32 @@
   <si>
     <t>pc.output_t</t>
   </si>
+  <si>
+    <t># industrial demand income elasticity as a function of per-capita industrial output</t>
+  </si>
+  <si>
+    <t># industrial demand income elasticity as a function of per-capita gdp</t>
+  </si>
+  <si>
+    <t>pc.output_GJ</t>
+  </si>
+  <si>
+    <t># aggregate buildings sector income elasticity as a function of per-capita gdp</t>
+  </si>
+  <si>
+    <t># aggregate transportation demand income elasticity as a function of per-capita gdp</t>
+  </si>
+  <si>
+    <t># cement demand income elasticity as a function of per-capita gdp</t>
+  </si>
+  <si>
+    <t># cement demand income elasticity as a function of per-capita cement output</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -323,7 +342,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="357">
+  <cellStyleXfs count="367">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -681,14 +700,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="357">
+  <cellStyles count="367">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -867,6 +895,11 @@
     <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1045,6 +1078,11 @@
     <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1612,11 +1650,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="442899304"/>
-        <c:axId val="442902312"/>
+        <c:axId val="508393016"/>
+        <c:axId val="412304488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="442899304"/>
+        <c:axId val="508393016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1626,12 +1664,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="442902312"/>
+        <c:crossAx val="412304488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="442902312"/>
+        <c:axId val="412304488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,7 +1680,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="442899304"/>
+        <c:crossAx val="508393016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2230,11 +2268,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="587781816"/>
-        <c:axId val="454893192"/>
+        <c:axId val="442173416"/>
+        <c:axId val="442183592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="587781816"/>
+        <c:axId val="442173416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2244,12 +2282,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="454893192"/>
+        <c:crossAx val="442183592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="454893192"/>
+        <c:axId val="442183592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2260,7 +2298,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="587781816"/>
+        <c:crossAx val="442173416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2424,11 +2462,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="587920456"/>
-        <c:axId val="588072104"/>
+        <c:axId val="508497688"/>
+        <c:axId val="442662168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="587920456"/>
+        <c:axId val="508497688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2437,7 +2475,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="588072104"/>
+        <c:crossAx val="442662168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2445,7 +2483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="588072104"/>
+        <c:axId val="442662168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2456,7 +2494,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="587920456"/>
+        <c:crossAx val="508497688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2614,11 +2652,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="454780184"/>
-        <c:axId val="587698488"/>
+        <c:axId val="451763192"/>
+        <c:axId val="442274840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="454780184"/>
+        <c:axId val="451763192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2627,7 +2665,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="587698488"/>
+        <c:crossAx val="442274840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2635,7 +2673,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="587698488"/>
+        <c:axId val="442274840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2646,7 +2684,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="454780184"/>
+        <c:crossAx val="451763192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3223,11 +3261,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="587525608"/>
-        <c:axId val="587528568"/>
+        <c:axId val="412209992"/>
+        <c:axId val="443081320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="587525608"/>
+        <c:axId val="412209992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3237,12 +3275,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="587528568"/>
+        <c:crossAx val="443081320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="587528568"/>
+        <c:axId val="443081320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3253,7 +3291,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="587525608"/>
+        <c:crossAx val="412209992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3417,11 +3455,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="587553528"/>
-        <c:axId val="587556536"/>
+        <c:axId val="508067288"/>
+        <c:axId val="442501128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="587553528"/>
+        <c:axId val="508067288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3430,7 +3468,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="587556536"/>
+        <c:crossAx val="442501128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3438,7 +3476,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="587556536"/>
+        <c:axId val="442501128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3449,7 +3487,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="587553528"/>
+        <c:crossAx val="508067288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4026,11 +4064,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="587595960"/>
-        <c:axId val="587598920"/>
+        <c:axId val="507560648"/>
+        <c:axId val="442506120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="587595960"/>
+        <c:axId val="507560648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4040,12 +4078,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="587598920"/>
+        <c:crossAx val="442506120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="587598920"/>
+        <c:axId val="442506120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4056,7 +4094,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="587595960"/>
+        <c:crossAx val="507560648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4220,11 +4258,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="587623832"/>
-        <c:axId val="587626840"/>
+        <c:axId val="507605864"/>
+        <c:axId val="442499464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="587623832"/>
+        <c:axId val="507605864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4233,7 +4271,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="587626840"/>
+        <c:crossAx val="442499464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4241,7 +4279,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="587626840"/>
+        <c:axId val="442499464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4252,7 +4290,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="587623832"/>
+        <c:crossAx val="507605864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4913,11 +4951,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="560686408"/>
-        <c:axId val="516534904"/>
+        <c:axId val="443447528"/>
+        <c:axId val="443387736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="560686408"/>
+        <c:axId val="443447528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4927,12 +4965,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="516534904"/>
+        <c:crossAx val="443387736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="516534904"/>
+        <c:axId val="443387736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4943,7 +4981,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="560686408"/>
+        <c:crossAx val="443447528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5531,11 +5569,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="455042776"/>
-        <c:axId val="587492456"/>
+        <c:axId val="442455944"/>
+        <c:axId val="479576456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="455042776"/>
+        <c:axId val="442455944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5545,12 +5583,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="587492456"/>
+        <c:crossAx val="479576456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="587492456"/>
+        <c:axId val="479576456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5561,7 +5599,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455042776"/>
+        <c:crossAx val="442455944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5725,11 +5763,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="455021192"/>
-        <c:axId val="587883080"/>
+        <c:axId val="441904792"/>
+        <c:axId val="441942664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="455021192"/>
+        <c:axId val="441904792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5738,7 +5776,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="587883080"/>
+        <c:crossAx val="441942664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5746,7 +5784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="587883080"/>
+        <c:axId val="441942664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5757,7 +5795,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="455021192"/>
+        <c:crossAx val="441904792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13355,6 +13393,155 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2.5</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>50</v>
+      </c>
+      <c r="B14">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>55</v>
+      </c>
+      <c r="B15">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>60</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23975,12 +24162,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -23990,121 +24177,126 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1.25</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>1.1000000000000001</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="B4">
-        <v>0.86</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>0.62</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B7">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B8">
-        <v>0.41</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B9">
-        <v>0.35</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B10">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B11">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B12">
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B13">
-        <v>0.12</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B14">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
+        <v>55</v>
+      </c>
+      <c r="B15">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
         <v>60</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>0</v>
       </c>
     </row>
@@ -24121,6 +24313,129 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>7.5</v>
+      </c>
+      <c r="B4">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>12.5</v>
+      </c>
+      <c r="B5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>17.5</v>
+      </c>
+      <c r="B6">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>45</v>
+      </c>
+      <c r="B9">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>65</v>
+      </c>
+      <c r="B10">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>95</v>
+      </c>
+      <c r="B11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>105</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>115</v>
+      </c>
+      <c r="B13">
+        <v>-0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W123"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
@@ -28255,9 +28570,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -28268,121 +28583,126 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0.9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>0.65</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="B4">
-        <v>0.56999999999999995</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>0.42499999999999999</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B7">
-        <v>0.36</v>
+        <v>0.42499999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B8">
-        <v>0.28999999999999998</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B9">
-        <v>0.22</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B10">
-        <v>0.18</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B11">
-        <v>0.14000000000000001</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B12">
-        <v>0.1</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B13">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
+        <v>55</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
         <v>60</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>-5.0000000000000001E-3</v>
       </c>
     </row>
@@ -28397,7 +28717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W121"/>
   <sheetViews>
@@ -32963,7 +33283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T180"/>
   <sheetViews>
@@ -36093,31 +36413,31 @@
         <v>12</v>
       </c>
       <c r="D66">
-        <f>LOG(N51,N20)</f>
+        <f t="shared" ref="D66:D79" si="29">LOG(N51,N20)</f>
         <v>4.7306539006595165E-4</v>
       </c>
       <c r="E66">
-        <f>LOG(O51,O20)</f>
+        <f t="shared" ref="E66:E79" si="30">LOG(O51,O20)</f>
         <v>-2.8053336836264701E-2</v>
       </c>
       <c r="F66">
-        <f>LOG(P51,P20)</f>
+        <f t="shared" ref="F66:F79" si="31">LOG(P51,P20)</f>
         <v>4.4823477464401949E-4</v>
       </c>
       <c r="G66">
-        <f>LOG(Q51,Q20)</f>
+        <f t="shared" ref="G66:G79" si="32">LOG(Q51,Q20)</f>
         <v>-1.6024993521401049E-2</v>
       </c>
       <c r="H66">
-        <f>LOG(R51,R20)</f>
+        <f t="shared" ref="H66:H79" si="33">LOG(R51,R20)</f>
         <v>7.8468697704888075E-3</v>
       </c>
       <c r="I66">
-        <f>LOG(S51,S20)</f>
+        <f t="shared" ref="I66:I79" si="34">LOG(S51,S20)</f>
         <v>-1.3019093751676144E-2</v>
       </c>
       <c r="J66">
-        <f>LOG(T51,T20)</f>
+        <f t="shared" ref="J66:J79" si="35">LOG(T51,T20)</f>
         <v>-1.2234563373649374E-2</v>
       </c>
     </row>
@@ -36132,31 +36452,31 @@
         <v>2</v>
       </c>
       <c r="D67">
-        <f>LOG(N52,N21)</f>
+        <f t="shared" si="29"/>
         <v>-0.29616911272593244</v>
       </c>
       <c r="E67">
-        <f>LOG(O52,O21)</f>
+        <f t="shared" si="30"/>
         <v>-0.12933111057051566</v>
       </c>
       <c r="F67">
-        <f>LOG(P52,P21)</f>
+        <f t="shared" si="31"/>
         <v>-8.9256392638190921E-2</v>
       </c>
       <c r="G67">
-        <f>LOG(Q52,Q21)</f>
+        <f t="shared" si="32"/>
         <v>-0.10919846211569534</v>
       </c>
       <c r="H67">
-        <f>LOG(R52,R21)</f>
+        <f t="shared" si="33"/>
         <v>3.1009091964973614E-2</v>
       </c>
       <c r="I67">
-        <f>LOG(S52,S21)</f>
+        <f t="shared" si="34"/>
         <v>0.12179670862640408</v>
       </c>
       <c r="J67">
-        <f>LOG(T52,T21)</f>
+        <f t="shared" si="35"/>
         <v>-0.28696134702683956</v>
       </c>
     </row>
@@ -36171,31 +36491,31 @@
         <v>13</v>
       </c>
       <c r="D68">
-        <f>LOG(N53,N22)</f>
+        <f t="shared" si="29"/>
         <v>-9.1404932068134659E-2</v>
       </c>
       <c r="E68">
-        <f>LOG(O53,O22)</f>
+        <f t="shared" si="30"/>
         <v>-0.10306127322836989</v>
       </c>
       <c r="F68">
-        <f>LOG(P53,P22)</f>
+        <f t="shared" si="31"/>
         <v>-8.9088188720467629E-2</v>
       </c>
       <c r="G68">
-        <f>LOG(Q53,Q22)</f>
+        <f t="shared" si="32"/>
         <v>-7.1134772487040851E-2</v>
       </c>
       <c r="H68">
-        <f>LOG(R53,R22)</f>
+        <f t="shared" si="33"/>
         <v>-3.9792916894415671E-2</v>
       </c>
       <c r="I68">
-        <f>LOG(S53,S22)</f>
+        <f t="shared" si="34"/>
         <v>-4.3468447361366506E-2</v>
       </c>
       <c r="J68">
-        <f>LOG(T53,T22)</f>
+        <f t="shared" si="35"/>
         <v>-2.1156404401738264E-2</v>
       </c>
     </row>
@@ -36210,31 +36530,31 @@
         <v>7</v>
       </c>
       <c r="D69">
-        <f>LOG(N54,N23)</f>
+        <f t="shared" si="29"/>
         <v>-0.11372648668097009</v>
       </c>
       <c r="E69">
-        <f>LOG(O54,O23)</f>
+        <f t="shared" si="30"/>
         <v>-1.50168928996758E-2</v>
       </c>
       <c r="F69">
-        <f>LOG(P54,P23)</f>
+        <f t="shared" si="31"/>
         <v>-1.8594367357092034E-2</v>
       </c>
       <c r="G69">
-        <f>LOG(Q54,Q23)</f>
+        <f t="shared" si="32"/>
         <v>-9.0652076630582445E-2</v>
       </c>
       <c r="H69">
-        <f>LOG(R54,R23)</f>
+        <f t="shared" si="33"/>
         <v>-4.2893082709937219E-2</v>
       </c>
       <c r="I69">
-        <f>LOG(S54,S23)</f>
+        <f t="shared" si="34"/>
         <v>2.7637684207346962E-2</v>
       </c>
       <c r="J69">
-        <f>LOG(T54,T23)</f>
+        <f t="shared" si="35"/>
         <v>-6.605622251014219E-2</v>
       </c>
     </row>
@@ -36249,31 +36569,31 @@
         <v>1</v>
       </c>
       <c r="D70">
-        <f>LOG(N55,N24)</f>
+        <f t="shared" si="29"/>
         <v>-0.1645334766845917</v>
       </c>
       <c r="E70">
-        <f>LOG(O55,O24)</f>
+        <f t="shared" si="30"/>
         <v>-0.15668035153243198</v>
       </c>
       <c r="F70">
-        <f>LOG(P55,P24)</f>
+        <f t="shared" si="31"/>
         <v>-0.14448472523076394</v>
       </c>
       <c r="G70">
-        <f>LOG(Q55,Q24)</f>
+        <f t="shared" si="32"/>
         <v>0.14851399385087899</v>
       </c>
       <c r="H70">
-        <f>LOG(R55,R24)</f>
+        <f t="shared" si="33"/>
         <v>0.14662778165123935</v>
       </c>
       <c r="I70">
-        <f>LOG(S55,S24)</f>
+        <f t="shared" si="34"/>
         <v>-0.3017296313250783</v>
       </c>
       <c r="J70">
-        <f>LOG(T55,T24)</f>
+        <f t="shared" si="35"/>
         <v>0.17688419318089252</v>
       </c>
     </row>
@@ -36288,31 +36608,31 @@
         <v>5</v>
       </c>
       <c r="D71">
-        <f>LOG(N56,N25)</f>
+        <f t="shared" si="29"/>
         <v>0.94063278992622201</v>
       </c>
       <c r="E71">
-        <f>LOG(O56,O25)</f>
+        <f t="shared" si="30"/>
         <v>0.85652005460974689</v>
       </c>
       <c r="F71">
-        <f>LOG(P56,P25)</f>
+        <f t="shared" si="31"/>
         <v>0.32774285585538732</v>
       </c>
       <c r="G71">
-        <f>LOG(Q56,Q25)</f>
+        <f t="shared" si="32"/>
         <v>-3.3567919356894758E-2</v>
       </c>
       <c r="H71">
-        <f>LOG(R56,R25)</f>
+        <f t="shared" si="33"/>
         <v>-7.0126678035935197E-2</v>
       </c>
       <c r="I71">
-        <f>LOG(S56,S25)</f>
+        <f t="shared" si="34"/>
         <v>-4.0934669387824127E-2</v>
       </c>
       <c r="J71">
-        <f>LOG(T56,T25)</f>
+        <f t="shared" si="35"/>
         <v>-1.0865727246856874E-2</v>
       </c>
     </row>
@@ -36327,31 +36647,31 @@
         <v>3</v>
       </c>
       <c r="D72">
-        <f>LOG(N57,N26)</f>
+        <f t="shared" si="29"/>
         <v>1.0137141780936658</v>
       </c>
       <c r="E72">
-        <f>LOG(O57,O26)</f>
+        <f t="shared" si="30"/>
         <v>0.89226930524657133</v>
       </c>
       <c r="F72">
-        <f>LOG(P57,P26)</f>
+        <f t="shared" si="31"/>
         <v>0.24448308432064553</v>
       </c>
       <c r="G72">
-        <f>LOG(Q57,Q26)</f>
+        <f t="shared" si="32"/>
         <v>-0.25179153065346932</v>
       </c>
       <c r="H72">
-        <f>LOG(R57,R26)</f>
+        <f t="shared" si="33"/>
         <v>-0.21902340295617548</v>
       </c>
       <c r="I72">
-        <f>LOG(S57,S26)</f>
+        <f t="shared" si="34"/>
         <v>-0.10283461523257317</v>
       </c>
       <c r="J72">
-        <f>LOG(T57,T26)</f>
+        <f t="shared" si="35"/>
         <v>-4.3355656781707469E-2</v>
       </c>
     </row>
@@ -36366,31 +36686,31 @@
         <v>10</v>
       </c>
       <c r="D73">
-        <f>LOG(N58,N27)</f>
+        <f t="shared" si="29"/>
         <v>1.0614348379644045</v>
       </c>
       <c r="E73">
-        <f>LOG(O58,O27)</f>
+        <f t="shared" si="30"/>
         <v>0.63184539959834907</v>
       </c>
       <c r="F73">
-        <f>LOG(P58,P27)</f>
+        <f t="shared" si="31"/>
         <v>0.10574150965887323</v>
       </c>
       <c r="G73">
-        <f>LOG(Q58,Q27)</f>
+        <f t="shared" si="32"/>
         <v>-9.0247514731603057E-2</v>
       </c>
       <c r="H73">
-        <f>LOG(R58,R27)</f>
+        <f t="shared" si="33"/>
         <v>-8.5344778967908111E-2</v>
       </c>
       <c r="I73">
-        <f>LOG(S58,S27)</f>
+        <f t="shared" si="34"/>
         <v>-4.998619702217922E-2</v>
       </c>
       <c r="J73">
-        <f>LOG(T58,T27)</f>
+        <f t="shared" si="35"/>
         <v>-3.6049028909220571E-2</v>
       </c>
     </row>
@@ -36405,31 +36725,31 @@
         <v>0</v>
       </c>
       <c r="D74">
-        <f>LOG(N59,N28)</f>
+        <f t="shared" si="29"/>
         <v>0.98481808448728303</v>
       </c>
       <c r="E74">
-        <f>LOG(O59,O28)</f>
+        <f t="shared" si="30"/>
         <v>1.0915957770985769</v>
       </c>
       <c r="F74">
-        <f>LOG(P59,P28)</f>
+        <f t="shared" si="31"/>
         <v>1.0814872618086075</v>
       </c>
       <c r="G74">
-        <f>LOG(Q59,Q28)</f>
+        <f t="shared" si="32"/>
         <v>0.65305279644284975</v>
       </c>
       <c r="H74">
-        <f>LOG(R59,R28)</f>
+        <f t="shared" si="33"/>
         <v>0.12493920237740018</v>
       </c>
       <c r="I74">
-        <f>LOG(S59,S28)</f>
+        <f t="shared" si="34"/>
         <v>-5.9831117922232641E-2</v>
       </c>
       <c r="J74">
-        <f>LOG(T59,T28)</f>
+        <f t="shared" si="35"/>
         <v>-5.9295661803926571E-2</v>
       </c>
     </row>
@@ -36444,31 +36764,31 @@
         <v>9</v>
       </c>
       <c r="D75">
-        <f>LOG(N60,N29)</f>
+        <f t="shared" si="29"/>
         <v>1.2772457944282707</v>
       </c>
       <c r="E75">
-        <f>LOG(O60,O29)</f>
+        <f t="shared" si="30"/>
         <v>0.96046995310247496</v>
       </c>
       <c r="F75">
-        <f>LOG(P60,P29)</f>
+        <f t="shared" si="31"/>
         <v>0.31886672099837765</v>
       </c>
       <c r="G75">
-        <f>LOG(Q60,Q29)</f>
+        <f t="shared" si="32"/>
         <v>2.3070016599723409E-2</v>
       </c>
       <c r="H75">
-        <f>LOG(R60,R29)</f>
+        <f t="shared" si="33"/>
         <v>-1.4745953606558193E-2</v>
       </c>
       <c r="I75">
-        <f>LOG(S60,S29)</f>
+        <f t="shared" si="34"/>
         <v>-1.3953641870109534E-2</v>
       </c>
       <c r="J75">
-        <f>LOG(T60,T29)</f>
+        <f t="shared" si="35"/>
         <v>-1.0726126612833503E-2</v>
       </c>
     </row>
@@ -36483,31 +36803,31 @@
         <v>11</v>
       </c>
       <c r="D76">
-        <f>LOG(N61,N30)</f>
+        <f t="shared" si="29"/>
         <v>1.0552973919664244</v>
       </c>
       <c r="E76">
-        <f>LOG(O61,O30)</f>
+        <f t="shared" si="30"/>
         <v>1.1011526165260979</v>
       </c>
       <c r="F76">
-        <f>LOG(P61,P30)</f>
+        <f t="shared" si="31"/>
         <v>0.96254632915073757</v>
       </c>
       <c r="G76">
-        <f>LOG(Q61,Q30)</f>
+        <f t="shared" si="32"/>
         <v>0.40402936198823436</v>
       </c>
       <c r="H76">
-        <f>LOG(R61,R30)</f>
+        <f t="shared" si="33"/>
         <v>1.1777418817757606E-2</v>
       </c>
       <c r="I76">
-        <f>LOG(S61,S30)</f>
+        <f t="shared" si="34"/>
         <v>-7.1398896007516838E-2</v>
       </c>
       <c r="J76">
-        <f>LOG(T61,T30)</f>
+        <f t="shared" si="35"/>
         <v>-4.9610488557913002E-2</v>
       </c>
     </row>
@@ -36522,31 +36842,31 @@
         <v>4</v>
       </c>
       <c r="D77">
-        <f>LOG(N62,N31)</f>
+        <f t="shared" si="29"/>
         <v>1.1141089864226463</v>
       </c>
       <c r="E77">
-        <f>LOG(O62,O31)</f>
+        <f t="shared" si="30"/>
         <v>0.77287180499315966</v>
       </c>
       <c r="F77">
-        <f>LOG(P62,P31)</f>
+        <f t="shared" si="31"/>
         <v>7.6454020877628995E-2</v>
       </c>
       <c r="G77">
-        <f>LOG(Q62,Q31)</f>
+        <f t="shared" si="32"/>
         <v>-4.745574390505479E-2</v>
       </c>
       <c r="H77">
-        <f>LOG(R62,R31)</f>
+        <f t="shared" si="33"/>
         <v>-6.5786677375637273E-2</v>
       </c>
       <c r="I77">
-        <f>LOG(S62,S31)</f>
+        <f t="shared" si="34"/>
         <v>-1.5074027787646478E-2</v>
       </c>
       <c r="J77">
-        <f>LOG(T62,T31)</f>
+        <f t="shared" si="35"/>
         <v>-5.4041019874204753E-2</v>
       </c>
     </row>
@@ -36561,31 +36881,31 @@
         <v>8</v>
       </c>
       <c r="D78">
-        <f>LOG(N63,N32)</f>
+        <f t="shared" si="29"/>
         <v>5.8216301405563178E-3</v>
       </c>
       <c r="E78">
-        <f>LOG(O63,O32)</f>
+        <f t="shared" si="30"/>
         <v>-0.19409587348943463</v>
       </c>
       <c r="F78">
-        <f>LOG(P63,P32)</f>
+        <f t="shared" si="31"/>
         <v>-3.877656332972871E-2</v>
       </c>
       <c r="G78">
-        <f>LOG(Q63,Q32)</f>
+        <f t="shared" si="32"/>
         <v>-5.1849492773038568E-2</v>
       </c>
       <c r="H78">
-        <f>LOG(R63,R32)</f>
+        <f t="shared" si="33"/>
         <v>4.2204225550374973E-2</v>
       </c>
       <c r="I78">
-        <f>LOG(S63,S32)</f>
+        <f t="shared" si="34"/>
         <v>-0.26615612560943874</v>
       </c>
       <c r="J78">
-        <f>LOG(T63,T32)</f>
+        <f t="shared" si="35"/>
         <v>0.20885679669136134</v>
       </c>
     </row>
@@ -36600,31 +36920,31 @@
         <v>6</v>
       </c>
       <c r="D79">
-        <f>LOG(N64,N33)</f>
+        <f t="shared" si="29"/>
         <v>1.1680764794877965</v>
       </c>
       <c r="E79">
-        <f>LOG(O64,O33)</f>
+        <f t="shared" si="30"/>
         <v>1.3595146567500096</v>
       </c>
       <c r="F79">
-        <f>LOG(P64,P33)</f>
+        <f t="shared" si="31"/>
         <v>1.3511719030165417</v>
       </c>
       <c r="G79">
-        <f>LOG(Q64,Q33)</f>
+        <f t="shared" si="32"/>
         <v>0.75752154397798743</v>
       </c>
       <c r="H79">
-        <f>LOG(R64,R33)</f>
+        <f t="shared" si="33"/>
         <v>0.22446388523341845</v>
       </c>
       <c r="I79">
-        <f>LOG(S64,S33)</f>
+        <f t="shared" si="34"/>
         <v>2.3460280763413621E-2</v>
       </c>
       <c r="J79">
-        <f>LOG(T64,T33)</f>
+        <f t="shared" si="35"/>
         <v>-4.5107815685697904E-3</v>
       </c>
     </row>
@@ -36668,11 +36988,11 @@
         <v>0</v>
       </c>
       <c r="J82">
-        <f t="shared" ref="J82:J93" si="29">I83</f>
+        <f t="shared" ref="J82:J91" si="36">I83</f>
         <v>0.1</v>
       </c>
       <c r="K82" t="str">
-        <f t="shared" ref="K82:K94" si="30">I82&amp;"-"&amp;J82</f>
+        <f t="shared" ref="K82:K91" si="37">I82&amp;"-"&amp;J82</f>
         <v>0-0.1</v>
       </c>
       <c r="L82">
@@ -36702,19 +37022,19 @@
         <v>1.1680764794877965</v>
       </c>
       <c r="I83" s="1">
-        <f>I82+0.1</f>
+        <f t="shared" ref="I83:I92" si="38">I82+0.1</f>
         <v>0.1</v>
       </c>
       <c r="J83">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>0.2</v>
       </c>
       <c r="K83" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>0.1-0.2</v>
       </c>
       <c r="L83">
-        <f t="shared" ref="L83:L91" si="31">AVERAGEIFS($H$83:$H$180,$G$83:$G$180,"&gt;"&amp;I83,$G$83:$G$180,"&lt;"&amp;J83)</f>
+        <f t="shared" ref="L83:L91" si="39">AVERAGEIFS($H$83:$H$180,$G$83:$G$180,"&gt;"&amp;I83,$G$83:$G$180,"&lt;"&amp;J83)</f>
         <v>1.0996249918647649</v>
       </c>
     </row>
@@ -36726,11 +37046,11 @@
         <v>2</v>
       </c>
       <c r="D84">
-        <f t="shared" ref="D84:D147" si="32">VLOOKUP($C84,$C$51:$K$64,MATCH($B84,$C$50:$K$50,0),FALSE)</f>
+        <f t="shared" ref="D84:D147" si="40">VLOOKUP($C84,$C$51:$K$64,MATCH($B84,$C$50:$K$50,0),FALSE)</f>
         <v>0.34482758620689657</v>
       </c>
       <c r="E84">
-        <f t="shared" ref="E84:E147" si="33">VLOOKUP($C84,$C$66:$K$79,MATCH($B84,$C$50:$K$50,0),FALSE)</f>
+        <f t="shared" ref="E84:E147" si="41">VLOOKUP($C84,$C$66:$K$79,MATCH($B84,$C$50:$K$50,0),FALSE)</f>
         <v>-0.29616911272593244</v>
       </c>
       <c r="G84">
@@ -36740,19 +37060,19 @@
         <v>1.3595146567500096</v>
       </c>
       <c r="I84" s="1">
-        <f>I83+0.1</f>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="J84">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="K84" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>0.2-0.3</v>
       </c>
       <c r="L84">
-        <f t="shared" si="31"/>
+        <f t="shared" si="39"/>
         <v>1.1088470929525656</v>
       </c>
     </row>
@@ -36764,11 +37084,11 @@
         <v>13</v>
       </c>
       <c r="D85">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.51833740831295838</v>
       </c>
       <c r="E85">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-9.1404932068134659E-2</v>
       </c>
       <c r="G85">
@@ -36778,19 +37098,19 @@
         <v>1.0552973919664244</v>
       </c>
       <c r="I85" s="1">
-        <f>I84+0.1</f>
+        <f t="shared" si="38"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="J85">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>0.4</v>
       </c>
       <c r="K85" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>0.3-0.4</v>
       </c>
       <c r="L85">
-        <f t="shared" si="31"/>
+        <f t="shared" si="39"/>
         <v>0.12378267647366091</v>
       </c>
     </row>
@@ -36802,11 +37122,11 @@
         <v>7</v>
       </c>
       <c r="D86">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.65891472868217049</v>
       </c>
       <c r="E86">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-0.11372648668097009</v>
       </c>
       <c r="G86">
@@ -36816,19 +37136,19 @@
         <v>0.98481808448728303</v>
       </c>
       <c r="I86" s="1">
-        <f>I85+0.1</f>
+        <f t="shared" si="38"/>
         <v>0.4</v>
       </c>
       <c r="J86">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>0.5</v>
       </c>
       <c r="K86" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>0.4-0.5</v>
       </c>
       <c r="L86">
-        <f t="shared" si="31"/>
+        <f t="shared" si="39"/>
         <v>0.33581389934075523</v>
       </c>
     </row>
@@ -36840,11 +37160,11 @@
         <v>1</v>
       </c>
       <c r="D87">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.38095238095238093</v>
       </c>
       <c r="E87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-0.1645334766845917</v>
       </c>
       <c r="G87">
@@ -36854,19 +37174,19 @@
         <v>1.0915957770985769</v>
       </c>
       <c r="I87" s="1">
-        <f>I86+0.1</f>
+        <f t="shared" si="38"/>
         <v>0.5</v>
       </c>
       <c r="J87">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>0.6</v>
       </c>
       <c r="K87" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>0.5-0.6</v>
       </c>
       <c r="L87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="39"/>
         <v>0.18010610312981887</v>
       </c>
     </row>
@@ -36878,11 +37198,11 @@
         <v>5</v>
       </c>
       <c r="D88">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.48780487804878048</v>
       </c>
       <c r="E88">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.94063278992622201</v>
       </c>
       <c r="G88">
@@ -36892,19 +37212,19 @@
         <v>1.1011526165260979</v>
       </c>
       <c r="I88" s="1">
-        <f>I87+0.1</f>
+        <f t="shared" si="38"/>
         <v>0.6</v>
       </c>
       <c r="J88">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>0.7</v>
       </c>
       <c r="K88" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>0.6-0.7</v>
       </c>
       <c r="L88">
-        <f t="shared" si="31"/>
+        <f t="shared" si="39"/>
         <v>-2.7233076938040786E-2</v>
       </c>
     </row>
@@ -36916,11 +37236,11 @@
         <v>3</v>
       </c>
       <c r="D89">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.18429752066115704</v>
       </c>
       <c r="E89">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>1.0137141780936658</v>
       </c>
       <c r="G89">
@@ -36930,19 +37250,19 @@
         <v>1.3511719030165417</v>
       </c>
       <c r="I89" s="1">
-        <f>I88+0.1</f>
+        <f t="shared" si="38"/>
         <v>0.7</v>
       </c>
       <c r="J89">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>0.79999999999999993</v>
       </c>
       <c r="K89" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>0.7-0.8</v>
       </c>
       <c r="L89">
-        <f t="shared" si="31"/>
+        <f t="shared" si="39"/>
         <v>-4.0703640496102068E-2</v>
       </c>
     </row>
@@ -36954,11 +37274,11 @@
         <v>10</v>
       </c>
       <c r="D90">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.4573643410852713</v>
       </c>
       <c r="E90">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>1.0614348379644045</v>
       </c>
       <c r="G90">
@@ -36968,19 +37288,19 @@
         <v>1.0137141780936658</v>
       </c>
       <c r="I90" s="1">
-        <f>I89+0.1</f>
+        <f t="shared" si="38"/>
         <v>0.79999999999999993</v>
       </c>
       <c r="J90">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="K90" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>0.8-0.9</v>
       </c>
       <c r="L90">
-        <f t="shared" si="31"/>
+        <f t="shared" si="39"/>
         <v>-0.25179153065346932</v>
       </c>
     </row>
@@ -36992,11 +37312,11 @@
         <v>0</v>
       </c>
       <c r="D91">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.11773700305810397</v>
       </c>
       <c r="E91">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.98481808448728303</v>
       </c>
       <c r="G91">
@@ -37006,19 +37326,19 @@
         <v>1.0814872618086075</v>
       </c>
       <c r="I91" s="1">
-        <f>I90+0.1</f>
+        <f t="shared" si="38"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="J91">
-        <f t="shared" si="29"/>
+        <f t="shared" si="36"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="K91" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="37"/>
         <v>0.9-1</v>
       </c>
       <c r="L91" t="e">
-        <f t="shared" si="31"/>
+        <f t="shared" si="39"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -37030,11 +37350,11 @@
         <v>9</v>
       </c>
       <c r="D92">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.23636363636363636</v>
       </c>
       <c r="E92">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>1.2772457944282707</v>
       </c>
       <c r="G92">
@@ -37044,7 +37364,7 @@
         <v>1.2772457944282707</v>
       </c>
       <c r="I92" s="1">
-        <f>I91+0.1</f>
+        <f t="shared" si="38"/>
         <v>0.99999999999999989</v>
       </c>
     </row>
@@ -37056,11 +37376,11 @@
         <v>11</v>
       </c>
       <c r="D93">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.10856269113149847</v>
       </c>
       <c r="E93">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>1.0552973919664244</v>
       </c>
       <c r="G93">
@@ -37079,11 +37399,11 @@
         <v>4</v>
       </c>
       <c r="D94">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.27049180327868855</v>
       </c>
       <c r="E94">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>1.1141089864226463</v>
       </c>
       <c r="G94">
@@ -37102,11 +37422,11 @@
         <v>8</v>
       </c>
       <c r="D95">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.76744186046511631</v>
       </c>
       <c r="E95">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>5.8216301405563178E-3</v>
       </c>
       <c r="G95">
@@ -37124,11 +37444,11 @@
         <v>6</v>
       </c>
       <c r="D96">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>4.700352526439483E-2</v>
       </c>
       <c r="E96">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>1.1680764794877965</v>
       </c>
       <c r="G96">
@@ -37146,11 +37466,11 @@
         <v>12</v>
       </c>
       <c r="D97">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.32534246575342468</v>
       </c>
       <c r="E97">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-2.8053336836264701E-2</v>
       </c>
       <c r="G97">
@@ -37168,11 +37488,11 @@
         <v>2</v>
       </c>
       <c r="D98">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.3235294117647059</v>
       </c>
       <c r="E98">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-0.12933111057051566</v>
       </c>
       <c r="G98">
@@ -37190,11 +37510,11 @@
         <v>13</v>
       </c>
       <c r="D99">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.50638297872340421</v>
       </c>
       <c r="E99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-0.10306127322836989</v>
       </c>
       <c r="G99">
@@ -37212,11 +37532,11 @@
         <v>7</v>
       </c>
       <c r="D100">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.64885496183206104</v>
       </c>
       <c r="E100">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-1.50168928996758E-2</v>
       </c>
       <c r="G100">
@@ -37234,11 +37554,11 @@
         <v>1</v>
       </c>
       <c r="D101">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="E101">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-0.15668035153243198</v>
       </c>
       <c r="G101">
@@ -37256,11 +37576,11 @@
         <v>5</v>
       </c>
       <c r="D102">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.37919463087248323</v>
       </c>
       <c r="E102">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.85652005460974689</v>
       </c>
       <c r="G102">
@@ -37278,11 +37598,11 @@
         <v>3</v>
       </c>
       <c r="D103">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.38227334235453314</v>
       </c>
       <c r="E103">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.89226930524657133</v>
       </c>
       <c r="G103">
@@ -37300,11 +37620,11 @@
         <v>10</v>
       </c>
       <c r="D104">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.48717948717948717</v>
       </c>
       <c r="E104">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.63184539959834907</v>
       </c>
       <c r="G104">
@@ -37322,11 +37642,11 @@
         <v>0</v>
       </c>
       <c r="D105">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.12203023758099352</v>
       </c>
       <c r="E105">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>1.0915957770985769</v>
       </c>
       <c r="G105">
@@ -37344,11 +37664,11 @@
         <v>9</v>
       </c>
       <c r="D106">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.30712979890310788</v>
       </c>
       <c r="E106">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.96046995310247496</v>
       </c>
       <c r="G106">
@@ -37366,11 +37686,11 @@
         <v>11</v>
       </c>
       <c r="D107">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.14733178654292342</v>
       </c>
       <c r="E107">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>1.1011526165260979</v>
       </c>
       <c r="G107">
@@ -37388,11 +37708,11 @@
         <v>4</v>
       </c>
       <c r="D108">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.35483870967741937</v>
       </c>
       <c r="E108">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.77287180499315966</v>
       </c>
       <c r="G108">
@@ -37410,11 +37730,11 @@
         <v>8</v>
       </c>
       <c r="D109">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.77083333333333337</v>
       </c>
       <c r="E109">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-0.19409587348943463</v>
       </c>
       <c r="G109">
@@ -37432,11 +37752,11 @@
         <v>6</v>
       </c>
       <c r="D110">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>7.0837166513339461E-2</v>
       </c>
       <c r="E110">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>1.3595146567500096</v>
       </c>
       <c r="G110">
@@ -37454,11 +37774,11 @@
         <v>12</v>
       </c>
       <c r="D111">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.32317073170731708</v>
       </c>
       <c r="E111">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>4.4823477464401949E-4</v>
       </c>
       <c r="G111">
@@ -37476,11 +37796,11 @@
         <v>2</v>
       </c>
       <c r="D112">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.31428571428571428</v>
       </c>
       <c r="E112">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-8.9256392638190921E-2</v>
       </c>
       <c r="G112">
@@ -37498,11 +37818,11 @@
         <v>13</v>
       </c>
       <c r="D113">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.493801652892562</v>
       </c>
       <c r="E113">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-8.9088188720467629E-2</v>
       </c>
       <c r="G113">
@@ -37520,11 +37840,11 @@
         <v>7</v>
       </c>
       <c r="D114">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.6470588235294118</v>
       </c>
       <c r="E114">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-1.8594367357092034E-2</v>
       </c>
       <c r="G114">
@@ -37542,11 +37862,11 @@
         <v>1</v>
       </c>
       <c r="D115">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.34782608695652173</v>
       </c>
       <c r="E115">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-0.14448472523076394</v>
       </c>
       <c r="G115">
@@ -37564,11 +37884,11 @@
         <v>5</v>
       </c>
       <c r="D116">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.56818181818181823</v>
       </c>
       <c r="E116">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.32774285585538732</v>
       </c>
       <c r="G116">
@@ -37586,11 +37906,11 @@
         <v>3</v>
       </c>
       <c r="D117">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.74499677211103943</v>
       </c>
       <c r="E117">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.24448308432064553</v>
       </c>
       <c r="G117">
@@ -37608,11 +37928,11 @@
         <v>10</v>
       </c>
       <c r="D118">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.6619718309859155</v>
       </c>
       <c r="E118">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.10574150965887323</v>
       </c>
       <c r="G118">
@@ -37630,11 +37950,11 @@
         <v>0</v>
       </c>
       <c r="D119">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.22395023328149299</v>
       </c>
       <c r="E119">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>1.0814872618086075</v>
       </c>
       <c r="G119">
@@ -37652,11 +37972,11 @@
         <v>9</v>
       </c>
       <c r="D120">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.52220520673813176</v>
       </c>
       <c r="E120">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.31886672099837765</v>
       </c>
       <c r="G120">
@@ -37674,11 +37994,11 @@
         <v>11</v>
       </c>
       <c r="D121">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.29080118694362017</v>
       </c>
       <c r="E121">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.96254632915073757</v>
       </c>
       <c r="G121">
@@ -37696,11 +38016,11 @@
         <v>4</v>
       </c>
       <c r="D122">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.63200000000000001</v>
       </c>
       <c r="E122">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>7.6454020877628995E-2</v>
       </c>
       <c r="G122">
@@ -37718,11 +38038,11 @@
         <v>8</v>
       </c>
       <c r="D123">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.66</v>
       </c>
       <c r="E123">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-3.877656332972871E-2</v>
       </c>
       <c r="G123">
@@ -37740,11 +38060,11 @@
         <v>6</v>
       </c>
       <c r="D124">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.16226415094339622</v>
       </c>
       <c r="E124">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>1.3511719030165417</v>
       </c>
       <c r="G124">
@@ -37762,11 +38082,11 @@
         <v>12</v>
       </c>
       <c r="D125">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.32320441988950277</v>
       </c>
       <c r="E125">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-1.6024993521401049E-2</v>
       </c>
       <c r="G125">
@@ -37784,11 +38104,11 @@
         <v>2</v>
       </c>
       <c r="D126">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.30769230769230771</v>
       </c>
       <c r="E126">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-0.10919846211569534</v>
       </c>
       <c r="G126">
@@ -37806,11 +38126,11 @@
         <v>13</v>
       </c>
       <c r="D127">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.48303393213572854</v>
       </c>
       <c r="E127">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-7.1134772487040851E-2</v>
       </c>
       <c r="G127">
@@ -37828,11 +38148,11 @@
         <v>7</v>
       </c>
       <c r="D128">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.64444444444444449</v>
       </c>
       <c r="E128">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-9.0652076630582445E-2</v>
       </c>
       <c r="G128">
@@ -37850,11 +38170,11 @@
         <v>1</v>
       </c>
       <c r="D129">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E129">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.14851399385087899</v>
       </c>
       <c r="G129">
@@ -37872,11 +38192,11 @@
         <v>5</v>
       </c>
       <c r="D130">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.67307692307692313</v>
       </c>
       <c r="E130">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-3.3567919356894758E-2</v>
       </c>
       <c r="G130">
@@ -37894,11 +38214,11 @@
         <v>3</v>
       </c>
       <c r="D131">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.87619047619047619</v>
       </c>
       <c r="E131">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-0.25179153065346932</v>
       </c>
       <c r="G131">
@@ -37916,11 +38236,11 @@
         <v>10</v>
       </c>
       <c r="D132">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.69696969696969702</v>
       </c>
       <c r="E132">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-9.0247514731603057E-2</v>
       </c>
       <c r="G132">
@@ -37938,11 +38258,11 @@
         <v>0</v>
       </c>
       <c r="D133">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.44339025932953829</v>
       </c>
       <c r="E133">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.65305279644284975</v>
       </c>
       <c r="G133">
@@ -37960,11 +38280,11 @@
         <v>9</v>
       </c>
       <c r="D134">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.62225274725274726</v>
       </c>
       <c r="E134">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>2.3070016599723409E-2</v>
       </c>
       <c r="G134">
@@ -37982,11 +38302,11 @@
         <v>11</v>
       </c>
       <c r="D135">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.55190771960958296</v>
       </c>
       <c r="E135">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.40402936198823436</v>
       </c>
       <c r="G135">
@@ -38004,11 +38324,11 @@
         <v>4</v>
       </c>
       <c r="D136">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E136">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-4.745574390505479E-2</v>
       </c>
       <c r="G136">
@@ -38026,11 +38346,11 @@
         <v>8</v>
       </c>
       <c r="D137">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.64583333333333337</v>
       </c>
       <c r="E137">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-5.1849492773038568E-2</v>
       </c>
       <c r="G137">
@@ -38048,11 +38368,11 @@
         <v>6</v>
       </c>
       <c r="D138">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.38690074274139097</v>
       </c>
       <c r="E138">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.75752154397798743</v>
       </c>
       <c r="G138">
@@ -38070,11 +38390,11 @@
         <v>12</v>
       </c>
       <c r="D139">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.32207792207792207</v>
       </c>
       <c r="E139">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>7.8468697704888075E-3</v>
       </c>
       <c r="G139">
@@ -38092,11 +38412,11 @@
         <v>2</v>
       </c>
       <c r="D140">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.3</v>
       </c>
       <c r="E140">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>3.1009091964973614E-2</v>
       </c>
       <c r="G140">
@@ -38114,11 +38434,11 @@
         <v>13</v>
       </c>
       <c r="D141">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.47494989979959917</v>
       </c>
       <c r="E141">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-3.9792916894415671E-2</v>
       </c>
       <c r="G141">
@@ -38136,11 +38456,11 @@
         <v>7</v>
       </c>
       <c r="D142">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.63157894736842102</v>
       </c>
       <c r="E142">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-4.2893082709937219E-2</v>
       </c>
       <c r="G142">
@@ -38158,11 +38478,11 @@
         <v>1</v>
       </c>
       <c r="D143">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.34782608695652173</v>
       </c>
       <c r="E143">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.14662778165123935</v>
       </c>
       <c r="G143">
@@ -38180,11 +38500,11 @@
         <v>5</v>
       </c>
       <c r="D144">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.66013071895424835</v>
       </c>
       <c r="E144">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-7.0126678035935197E-2</v>
       </c>
       <c r="G144">
@@ -38202,11 +38522,11 @@
         <v>3</v>
       </c>
       <c r="D145">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.76980365605958023</v>
       </c>
       <c r="E145">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-0.21902340295617548</v>
       </c>
       <c r="G145">
@@ -38224,11 +38544,11 @@
         <v>10</v>
       </c>
       <c r="D146">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.66436781609195406</v>
       </c>
       <c r="E146">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>-8.5344778967908111E-2</v>
       </c>
       <c r="G146">
@@ -38246,11 +38566,11 @@
         <v>0</v>
       </c>
       <c r="D147">
-        <f t="shared" si="32"/>
+        <f t="shared" si="40"/>
         <v>0.64148877941981386</v>
       </c>
       <c r="E147">
-        <f t="shared" si="33"/>
+        <f t="shared" si="41"/>
         <v>0.12493920237740018</v>
       </c>
       <c r="G147">
@@ -38268,11 +38588,11 @@
         <v>9</v>
       </c>
       <c r="D148">
-        <f t="shared" ref="D148:D180" si="34">VLOOKUP($C148,$C$51:$K$64,MATCH($B148,$C$50:$K$50,0),FALSE)</f>
+        <f t="shared" ref="D148:D180" si="42">VLOOKUP($C148,$C$51:$K$64,MATCH($B148,$C$50:$K$50,0),FALSE)</f>
         <v>0.63102998696219037</v>
       </c>
       <c r="E148">
-        <f t="shared" ref="E148:E180" si="35">VLOOKUP($C148,$C$66:$K$79,MATCH($B148,$C$50:$K$50,0),FALSE)</f>
+        <f t="shared" ref="E148:E180" si="43">VLOOKUP($C148,$C$66:$K$79,MATCH($B148,$C$50:$K$50,0),FALSE)</f>
         <v>-1.4745953606558193E-2</v>
       </c>
       <c r="G148">
@@ -38290,11 +38610,11 @@
         <v>11</v>
       </c>
       <c r="D149">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="E149">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>1.1777418817757606E-2</v>
       </c>
       <c r="G149">
@@ -38312,11 +38632,11 @@
         <v>4</v>
       </c>
       <c r="D150">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.64655172413793105</v>
       </c>
       <c r="E150">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-6.5786677375637273E-2</v>
       </c>
       <c r="G150">
@@ -38334,11 +38654,11 @@
         <v>8</v>
       </c>
       <c r="D151">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.63636363636363635</v>
       </c>
       <c r="E151">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>4.2204225550374973E-2</v>
       </c>
       <c r="G151">
@@ -38356,11 +38676,11 @@
         <v>6</v>
       </c>
       <c r="D152">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.54996776273372017</v>
       </c>
       <c r="E152">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>0.22446388523341845</v>
       </c>
       <c r="G152">
@@ -38378,11 +38698,11 @@
         <v>12</v>
       </c>
       <c r="D153">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.32266009852216748</v>
       </c>
       <c r="E153">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-1.3019093751676144E-2</v>
       </c>
       <c r="G153">
@@ -38400,11 +38720,11 @@
         <v>2</v>
       </c>
       <c r="D154">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.30232558139534882</v>
       </c>
       <c r="E154">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>0.12179670862640408</v>
       </c>
       <c r="G154">
@@ -38422,11 +38742,11 @@
         <v>13</v>
       </c>
       <c r="D155">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.47022587268993837</v>
       </c>
       <c r="E155">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-4.3468447361366506E-2</v>
       </c>
       <c r="G155">
@@ -38444,11 +38764,11 @@
         <v>7</v>
       </c>
       <c r="D156">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.625</v>
       </c>
       <c r="E156">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>2.7637684207346962E-2</v>
       </c>
       <c r="G156">
@@ -38466,11 +38786,11 @@
         <v>1</v>
       </c>
       <c r="D157">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="E157">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-0.3017296313250783</v>
       </c>
       <c r="G157">
@@ -38488,11 +38808,11 @@
         <v>5</v>
       </c>
       <c r="D158">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.63822525597269619</v>
       </c>
       <c r="E158">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-4.0934669387824127E-2</v>
       </c>
       <c r="G158">
@@ -38510,11 +38830,11 @@
         <v>3</v>
       </c>
       <c r="D159">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.67555217060167561</v>
       </c>
       <c r="E159">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-0.10283461523257317</v>
       </c>
       <c r="G159">
@@ -38532,11 +38852,11 @@
         <v>10</v>
       </c>
       <c r="D160">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.64462809917355368</v>
       </c>
       <c r="E160">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-4.998619702217922E-2</v>
       </c>
       <c r="G160">
@@ -38554,11 +38874,11 @@
         <v>0</v>
       </c>
       <c r="D161">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.67654573326520184</v>
       </c>
       <c r="E161">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-5.9831117922232641E-2</v>
       </c>
       <c r="G161">
@@ -38576,11 +38896,11 @@
         <v>9</v>
       </c>
       <c r="D162">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.62729658792650922</v>
       </c>
       <c r="E162">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-1.3953641870109534E-2</v>
       </c>
       <c r="G162">
@@ -38598,11 +38918,11 @@
         <v>11</v>
       </c>
       <c r="D163">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.67045454545454541</v>
       </c>
       <c r="E163">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-7.1398896007516838E-2</v>
       </c>
       <c r="G163">
@@ -38620,11 +38940,11 @@
         <v>4</v>
       </c>
       <c r="D164">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.62962962962962965</v>
       </c>
       <c r="E164">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-1.5074027787646478E-2</v>
       </c>
       <c r="G164">
@@ -38642,11 +38962,11 @@
         <v>8</v>
       </c>
       <c r="D165">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.6428571428571429</v>
       </c>
       <c r="E165">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-0.26615612560943874</v>
       </c>
       <c r="G165">
@@ -38664,11 +38984,11 @@
         <v>6</v>
       </c>
       <c r="D166">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.61644736842105263</v>
       </c>
       <c r="E166">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>2.3460280763413621E-2</v>
       </c>
       <c r="G166">
@@ -38686,11 +39006,11 @@
         <v>12</v>
       </c>
       <c r="D167">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.32175925925925924</v>
       </c>
       <c r="E167">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-1.2234563373649374E-2</v>
       </c>
       <c r="G167">
@@ -38708,11 +39028,11 @@
         <v>2</v>
       </c>
       <c r="D168">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.31111111111111112</v>
       </c>
       <c r="E168">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-0.28696134702683956</v>
       </c>
       <c r="G168">
@@ -38730,11 +39050,11 @@
         <v>13</v>
       </c>
       <c r="D169">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.46540880503144655</v>
       </c>
       <c r="E169">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-2.1156404401738264E-2</v>
       </c>
       <c r="G169">
@@ -38752,11 +39072,11 @@
         <v>7</v>
       </c>
       <c r="D170">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.62903225806451613</v>
       </c>
       <c r="E170">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-6.605622251014219E-2</v>
       </c>
       <c r="G170">
@@ -38774,11 +39094,11 @@
         <v>1</v>
       </c>
       <c r="D171">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E171">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>0.17688419318089252</v>
       </c>
       <c r="G171">
@@ -38796,11 +39116,11 @@
         <v>5</v>
       </c>
       <c r="D172">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.62681159420289856</v>
       </c>
       <c r="E172">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-1.0865727246856874E-2</v>
       </c>
       <c r="G172">
@@ -38818,11 +39138,11 @@
         <v>3</v>
       </c>
       <c r="D173">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.64171122994652408</v>
       </c>
       <c r="E173">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-4.3355656781707469E-2</v>
       </c>
       <c r="G173">
@@ -38840,11 +39160,11 @@
         <v>10</v>
       </c>
       <c r="D174">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.63492063492063489</v>
       </c>
       <c r="E174">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-3.6049028909220571E-2</v>
       </c>
       <c r="G174">
@@ -38862,11 +39182,11 @@
         <v>0</v>
       </c>
       <c r="D175">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.65474974463738511</v>
       </c>
       <c r="E175">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-5.9295661803926571E-2</v>
       </c>
       <c r="G175">
@@ -38884,11 +39204,11 @@
         <v>9</v>
       </c>
       <c r="D176">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.62430939226519333</v>
       </c>
       <c r="E176">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-1.0726126612833503E-2</v>
       </c>
       <c r="G176">
@@ -38906,11 +39226,11 @@
         <v>11</v>
       </c>
       <c r="D177">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.64666666666666661</v>
       </c>
       <c r="E177">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-4.9610488557913002E-2</v>
       </c>
       <c r="G177">
@@ -38928,11 +39248,11 @@
         <v>4</v>
       </c>
       <c r="D178">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.6262626262626263</v>
       </c>
       <c r="E178">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-5.4041019874204753E-2</v>
       </c>
       <c r="G178">
@@ -38950,11 +39270,11 @@
         <v>8</v>
       </c>
       <c r="D179">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.6097560975609756</v>
       </c>
       <c r="E179">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>0.20885679669136134</v>
       </c>
       <c r="G179">
@@ -38972,11 +39292,11 @@
         <v>6</v>
       </c>
       <c r="D180">
-        <f t="shared" si="34"/>
+        <f t="shared" si="42"/>
         <v>0.625</v>
       </c>
       <c r="E180">
-        <f t="shared" si="35"/>
+        <f t="shared" si="43"/>
         <v>-4.5107815685697904E-3</v>
       </c>
       <c r="G180">
@@ -39001,12 +39321,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -39016,226 +39336,87 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>80</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1.263795568118903</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>0.1</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1.0996249918647649</v>
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1.264</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>0.2</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1.1088470929525656</v>
+        <v>0.1</v>
+      </c>
+      <c r="B4">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0.6</v>
+        <v>0.2</v>
+      </c>
+      <c r="B5">
+        <v>1.109</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>0.4</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.33581389934075523</v>
+        <v>0.3</v>
+      </c>
+      <c r="B6">
+        <v>0.6</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>0.5</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.18010610312981887</v>
+        <v>0.4</v>
+      </c>
+      <c r="B7">
+        <v>0.33600000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>0.6</v>
-      </c>
-      <c r="B8" s="3">
-        <v>-2.7233076938040786E-2</v>
+        <v>0.5</v>
+      </c>
+      <c r="B8">
+        <v>0.18</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>0.7</v>
-      </c>
-      <c r="B9" s="3">
-        <v>-4.0703640496102068E-2</v>
+        <v>0.6</v>
+      </c>
+      <c r="B9">
+        <v>-2.7E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>0.79999999999999993</v>
-      </c>
-      <c r="B10" s="3">
-        <v>-0.25179153065346932</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2.5</v>
-      </c>
-      <c r="B3">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>20</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>25</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>30</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>35</v>
+        <v>0.7</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>-4.1000000000000002E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>40</v>
+        <v>0.8</v>
       </c>
       <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>45</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>50</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>55</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
-        <v>60</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
+        <v>-0.252</v>
       </c>
     </row>
   </sheetData>
@@ -39251,6 +39432,155 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2.5</v>
+      </c>
+      <c r="B4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>50</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>55</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>60</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X225"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -51731,148 +52061,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2.5</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>20</v>
-      </c>
-      <c r="B7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>25</v>
-      </c>
-      <c r="B8">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9">
-        <v>30</v>
-      </c>
-      <c r="B9">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
-        <v>35</v>
-      </c>
-      <c r="B10">
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
-        <v>40</v>
-      </c>
-      <c r="B11">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12">
-        <v>45</v>
-      </c>
-      <c r="B12">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13">
-        <v>50</v>
-      </c>
-      <c r="B13">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14">
-        <v>55</v>
-      </c>
-      <c r="B14">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15">
-        <v>60</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>